<commit_message>
🔒 Added role-based access controls and cleaned up page logic
</commit_message>
<xml_diff>
--- a/Dispatch_Summary.xlsx
+++ b/Dispatch_Summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="60">
   <si>
     <t>Order ID</t>
   </si>
@@ -49,13 +49,40 @@
     <t>Dispatched By</t>
   </si>
   <si>
+    <t>madhu</t>
+  </si>
+  <si>
+    <t>aakarsh</t>
+  </si>
+  <si>
+    <t>praveen &amp; co</t>
+  </si>
+  <si>
+    <t>Madhu123</t>
+  </si>
+  <si>
+    <t>pkc</t>
+  </si>
+  <si>
     <t>amit</t>
   </si>
   <si>
     <t>Amit Jawla</t>
   </si>
   <si>
-    <t>praveen &amp; co</t>
+    <t>black salt</t>
+  </si>
+  <si>
+    <t>sendha namak</t>
+  </si>
+  <si>
+    <t>MTV Rock salt</t>
+  </si>
+  <si>
+    <t>rock salt</t>
+  </si>
+  <si>
+    <t>cheetah salt</t>
   </si>
   <si>
     <t>Virat rock Salt</t>
@@ -64,7 +91,13 @@
     <t>Chheta</t>
   </si>
   <si>
-    <t>MTV Rock salt</t>
+    <t>100 KG</t>
+  </si>
+  <si>
+    <t>10 kg</t>
+  </si>
+  <si>
+    <t>1 KG</t>
   </si>
   <si>
     <t>1000 KG</t>
@@ -79,21 +112,45 @@
     <t>100 kg</t>
   </si>
   <si>
-    <t>10 kg</t>
+    <t>35.0 INR</t>
+  </si>
+  <si>
+    <t>22.0 INR</t>
+  </si>
+  <si>
+    <t>None None</t>
+  </si>
+  <si>
+    <t>0.0 INR</t>
+  </si>
+  <si>
+    <t>11.0 INR</t>
   </si>
   <si>
     <t>10.0 INR</t>
   </si>
   <si>
-    <t>11.0 INR</t>
-  </si>
-  <si>
-    <t>None None</t>
-  </si>
-  <si>
     <t>Per KG</t>
   </si>
   <si>
+    <t>29-04-2025 02:21 PM</t>
+  </si>
+  <si>
+    <t>29-04-2025 02:10 PM</t>
+  </si>
+  <si>
+    <t>28-04-2025 04:26 PM</t>
+  </si>
+  <si>
+    <t>28-04-2025 07:27 PM</t>
+  </si>
+  <si>
+    <t>29-04-2025 09:54 AM</t>
+  </si>
+  <si>
+    <t>29-04-2025 08:35 AM</t>
+  </si>
+  <si>
     <t>28-04-2025 06:37 PM</t>
   </si>
   <si>
@@ -112,6 +169,15 @@
     <t>28-04-2025 03:58 PM</t>
   </si>
   <si>
+    <t>29-04-2025 02:45 PM</t>
+  </si>
+  <si>
+    <t>29-04-2025 10:10 AM</t>
+  </si>
+  <si>
+    <t>29-04-2025 10:09 AM</t>
+  </si>
+  <si>
     <t>28-04-2025 06:48 PM</t>
   </si>
   <si>
@@ -121,7 +187,13 @@
     <t>28-04-2025 04:36 PM</t>
   </si>
   <si>
+    <t>vishal.sharma</t>
+  </si>
+  <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>ajay.sharma</t>
   </si>
 </sst>
 </file>
@@ -479,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -522,194 +594,424 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="K4" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="K5" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>35</v>
+        <v>58</v>
+      </c>
+      <c r="K6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
         <v>34</v>
       </c>
-      <c r="J7" t="s">
-        <v>35</v>
+      <c r="H14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>